<commit_message>
Made changes to allow for proper testing
</commit_message>
<xml_diff>
--- a/Assignments/Assignment3/Benchmarks.xlsx
+++ b/Assignments/Assignment3/Benchmarks.xlsx
@@ -1,31 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
-  <workbookPr checkCompatibility="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitty/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarioMan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20540" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Notes" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$59</definedName>
-  </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,49 +25,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Non-blocking</t>
+    <t>1-32 threads</t>
   </si>
   <si>
-    <t>Blocking</t>
+    <t>10000 key range</t>
   </si>
   <si>
-    <t>Times are reported in milliseconds.</t>
+    <t>Ratios</t>
   </si>
   <si>
-    <t>Notes:</t>
+    <t>Mixed</t>
   </si>
   <si>
-    <t>Test 3</t>
+    <t>Write-dominated</t>
   </si>
   <si>
-    <t>Test 1 (mixed)</t>
+    <t>Read-dominated</t>
   </si>
   <si>
-    <t>Test 2 (write-dominated)</t>
+    <t>Transaction sizes: 1, 2, 4, 8</t>
   </si>
   <si>
-    <t>Computed using 2.9GHz quad-core Intel i5 (4 cores, 4 logical processors)</t>
+    <t>Insert</t>
   </si>
   <si>
-    <t xml:space="preserve">200000 operations evenly divided between threads. </t>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Find</t>
+  </si>
+  <si>
+    <t>Mixed (33-33-33)</t>
+  </si>
+  <si>
+    <t>Write-dominated (33-50-0)</t>
+  </si>
+  <si>
+    <t>Read-dominated (15-5-80)</t>
+  </si>
+  <si>
+    <t>100000 transactions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -112,47 +113,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -166,7 +142,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -199,16 +175,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Test 1</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Mixed</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -249,11 +221,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Data!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-blocking</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -268,72 +240,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:f>Data!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Data!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>51910.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>26894.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15142.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15106.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14732.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14930.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14892.0</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4187-4D12-B12F-F029BDB4CAEA}"/>
+              <c16:uniqueId val="{00000000-F16E-4CDD-AA0D-3149DE208A5D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -342,11 +302,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Data!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Blocking</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -361,72 +321,222 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:f>Data!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:f>Data!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>33161.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>36705.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>36364.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>36121.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>36353.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>36349.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>36492.0</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4187-4D12-B12F-F029BDB4CAEA}"/>
+              <c16:uniqueId val="{00000001-F16E-4CDD-AA0D-3149DE208A5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F16E-4CDD-AA0D-3149DE208A5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$E$3:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F16E-4CDD-AA0D-3149DE208A5D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -438,12 +548,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1501180080"/>
-        <c:axId val="-1501169344"/>
+        <c:axId val="475928344"/>
+        <c:axId val="475929984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1501180080"/>
+        <c:axId val="475928344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -470,12 +581,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Threads</a:t>
+                  <a:t>Thread Count</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -542,7 +652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1501169344"/>
+        <c:crossAx val="475929984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -550,7 +660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1501169344"/>
+        <c:axId val="475929984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -591,12 +701,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Milliseconds</a:t>
+                  <a:t>Committed Transactions</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -657,7 +766,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1501180080"/>
+        <c:crossAx val="475928344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -671,7 +780,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -739,7 +847,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -772,16 +880,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Test 2</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Write-Dominated</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -818,15 +922,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Data!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-blocking</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -841,85 +945,73 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:f>Data!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$9</c:f>
+              <c:f>Data!$F$3:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>83262.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43065.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>23733.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23784.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>23481.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>24023.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>23915.0</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-B711-4337-99C0-5C0AA8F87EB2}"/>
+              <c16:uniqueId val="{00000000-5445-451B-AF50-634FF4381556}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Data!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Blocking</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -934,72 +1026,222 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:f>Data!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$9</c:f>
+              <c:f>Data!$G$3:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>54276.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>57271.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>56791.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>57115.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>57635.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>57161.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>59209.0</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B711-4337-99C0-5C0AA8F87EB2}"/>
+              <c16:uniqueId val="{00000001-5445-451B-AF50-634FF4381556}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5445-451B-AF50-634FF4381556}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$3:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5445-451B-AF50-634FF4381556}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1011,12 +1253,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1501021360"/>
-        <c:axId val="-1501012688"/>
+        <c:axId val="475928344"/>
+        <c:axId val="475929984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1501021360"/>
+        <c:axId val="475928344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1042,16 +1285,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Threads</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Thread Count</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1118,7 +1357,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1501012688"/>
+        <c:crossAx val="475929984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1126,7 +1365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1501012688"/>
+        <c:axId val="475929984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1167,12 +1406,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Milliseconds</a:t>
+                  <a:t>Committed Transactions</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1233,7 +1471,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1501021360"/>
+        <c:crossAx val="475928344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1247,7 +1485,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1315,7 +1552,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1348,15 +1585,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Test 3</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Read-Dominated</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1397,11 +1631,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
+              <c:f>Data!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-blocking</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1416,72 +1650,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:f>Data!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$9</c:f>
+              <c:f>Data!$J$3:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>84593.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43655.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>24052.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23893.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>23717.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>23794.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>23706.0</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9524-4C67-AB89-EA8C836DCE0E}"/>
+              <c16:uniqueId val="{00000000-45C8-464E-AA4A-35D80A11E5BF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1490,11 +1712,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Data!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Blocking</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1509,72 +1731,222 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:f>Data!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$9</c:f>
+              <c:f>Data!$K$3:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>57281.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>57471.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>57814.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>58630.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>59230.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>61837.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>61390.0</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9524-4C67-AB89-EA8C836DCE0E}"/>
+              <c16:uniqueId val="{00000001-45C8-464E-AA4A-35D80A11E5BF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$L$3:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-45C8-464E-AA4A-35D80A11E5BF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$M$3:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-45C8-464E-AA4A-35D80A11E5BF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1586,12 +1958,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1500288816"/>
-        <c:axId val="-1500280288"/>
+        <c:axId val="475928344"/>
+        <c:axId val="475929984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1500288816"/>
+        <c:axId val="475928344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,16 +1990,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Threads</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Thread Count</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1693,7 +2062,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1500280288"/>
+        <c:crossAx val="475929984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1701,7 +2070,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1500280288"/>
+        <c:axId val="475929984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1742,12 +2111,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Milliseconds</a:t>
+                  <a:t>Committed Transactions</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1808,7 +2176,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1500288816"/>
+        <c:crossAx val="475928344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1822,7 +2190,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2010,7 +2377,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2118,11 +2485,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2133,11 +2495,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2169,9 +2526,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2526,7 +2880,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2634,11 +2988,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2649,11 +2998,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2685,9 +3029,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3042,7 +3383,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3150,11 +3491,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3165,11 +3501,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3201,9 +3532,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3561,23 +3889,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A412E19D-B20A-41EB-A58B-725CBE836FBA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7C3212F-DFA1-4EBD-B3B8-7E61293086D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3597,27 +3925,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3E6CC3BE-C2A4-4E52-968C-68380AAB30F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{972C2A70-B0DD-46B8-9BBB-89638D2B822A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3633,23 +3963,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7352A349-1BFE-44F9-B3C1-B344D36D89CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AF59F90-DE38-4294-B629-87A81B714F03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3969,255 +4299,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3">
+        <v>3</v>
+      </c>
+      <c r="I2" s="3">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2</v>
+      </c>
+      <c r="L2" s="3">
+        <v>3</v>
+      </c>
+      <c r="M2" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>1</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
-      <c r="B3" s="2">
-        <v>51910</v>
+      <c r="D4" t="s">
+        <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>33161</v>
-      </c>
-      <c r="D3" s="2">
-        <v>83262</v>
-      </c>
-      <c r="E3" s="2">
-        <v>54276</v>
-      </c>
-      <c r="F3" s="2">
-        <v>84593</v>
-      </c>
-      <c r="G3" s="2">
-        <v>57281</v>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>26894</v>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
-      <c r="C4" s="2">
-        <v>36705</v>
+      <c r="C5" s="1">
+        <v>0.33</v>
       </c>
-      <c r="D4" s="2">
-        <v>43065</v>
+      <c r="D5" s="1">
+        <v>0.33</v>
       </c>
-      <c r="E4" s="2">
-        <v>57271</v>
-      </c>
-      <c r="F4" s="2">
-        <v>43655</v>
-      </c>
-      <c r="G4" s="2">
-        <v>57471</v>
+      <c r="E5" s="1">
+        <v>0.33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>15142</v>
+      <c r="C6" s="1">
+        <v>0.33</v>
       </c>
-      <c r="C5" s="2">
-        <v>36364</v>
+      <c r="D6" s="1">
+        <v>0.5</v>
       </c>
-      <c r="D5" s="2">
-        <v>23733</v>
-      </c>
-      <c r="E5" s="2">
-        <v>56791</v>
-      </c>
-      <c r="F5" s="2">
-        <v>24052</v>
-      </c>
-      <c r="G5" s="2">
-        <v>57814</v>
+      <c r="E6" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>8</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>15106</v>
+      <c r="C7" s="1">
+        <v>0.15</v>
       </c>
-      <c r="C6" s="2">
-        <v>36121</v>
+      <c r="D7" s="1">
+        <v>0.05</v>
       </c>
-      <c r="D6" s="2">
-        <v>23784</v>
-      </c>
-      <c r="E6" s="2">
-        <v>57115</v>
-      </c>
-      <c r="F6" s="2">
-        <v>23893</v>
-      </c>
-      <c r="G6" s="2">
-        <v>58630</v>
+      <c r="E7" s="1">
+        <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2">
-        <v>14732</v>
-      </c>
-      <c r="C7" s="2">
-        <v>36353</v>
-      </c>
-      <c r="D7" s="2">
-        <v>23481</v>
-      </c>
-      <c r="E7" s="2">
-        <v>57635</v>
-      </c>
-      <c r="F7" s="2">
-        <v>23717</v>
-      </c>
-      <c r="G7" s="2">
-        <v>59230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2">
-        <v>14930</v>
-      </c>
-      <c r="C8" s="2">
-        <v>36349</v>
-      </c>
-      <c r="D8" s="2">
-        <v>24023</v>
-      </c>
-      <c r="E8" s="2">
-        <v>57161</v>
-      </c>
-      <c r="F8" s="2">
-        <v>23794</v>
-      </c>
-      <c r="G8" s="2">
-        <v>61837</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>64</v>
-      </c>
-      <c r="B9" s="2">
-        <v>14892</v>
-      </c>
-      <c r="C9" s="2">
-        <v>36492</v>
-      </c>
-      <c r="D9" s="2">
-        <v>23915</v>
-      </c>
-      <c r="E9" s="2">
-        <v>59209</v>
-      </c>
-      <c r="F9" s="2">
-        <v>23706</v>
-      </c>
-      <c r="G9" s="2">
-        <v>61390</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>7</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B3:G9">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"DNF"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="77" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated benchmarks to display ops/sec
</commit_message>
<xml_diff>
--- a/Assignments/Assignment3/Benchmarks.xlsx
+++ b/Assignments/Assignment3/Benchmarks.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
-    <sheet name="Notes" sheetId="1" r:id="rId2"/>
+    <sheet name="Raw Data" sheetId="3" r:id="rId2"/>
+    <sheet name="Notes" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Data!$A$1:$M$59</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>1-32 threads</t>
   </si>
@@ -78,10 +79,22 @@
     <t xml:space="preserve">Computed using Intel i7-6700K@4.00GHz (4 physical, 8 logical) </t>
   </si>
   <si>
-    <t>320000 transactions</t>
+    <t>10,000 key range</t>
   </si>
   <si>
-    <t>Read dominated 4 operatrions per transaction had 0 successes, but is reported as 1 so the line shows on the graph</t>
+    <t>320,000 transactions</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>Commits</t>
+  </si>
+  <si>
+    <t>Ops/sec</t>
+  </si>
+  <si>
+    <t>Read dominated 4 operatrions per transaction had 0 successes, so it cannot appear on the logarithmic graph</t>
   </si>
 </sst>
 </file>
@@ -277,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -298,12 +311,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -475,22 +489,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3746</c:v>
+                  <c:v>1.0943286193322642E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3661</c:v>
+                  <c:v>2.1766045669567249E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3707</c:v>
+                  <c:v>4.1319638271742769E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3760</c:v>
+                  <c:v>5.9228295819935696E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3727</c:v>
+                  <c:v>6.0121192269898464E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3719</c:v>
+                  <c:v>6.1241065627030543E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -574,22 +588,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>194</c:v>
+                  <c:v>5.6526504008767373E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>208</c:v>
+                  <c:v>1.277550785521091E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>2.3294143500714208E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>180</c:v>
+                  <c:v>3.0574428659666461E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>214</c:v>
+                  <c:v>3.2617218127646231E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>187</c:v>
+                  <c:v>3.5912919116478629E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -673,22 +687,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>4.5722123792650169E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>8.6137590444469967E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>2.6645942045076053E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>3.2185387833923397E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>2.3151720944590216E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>2.6459143968871595E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -772,22 +786,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>8.5918034195377605E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>1.7029006073678833E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>2.2070183182520415E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>3.2690421706440012E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>6.449532408900355E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>1.6020506247997438E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -961,7 +975,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Committed Transactions</a:t>
+                  <a:t>Ops/sec</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1253,22 +1267,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3690</c:v>
+                  <c:v>9.5716471188169296E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3753</c:v>
+                  <c:v>1.9041523731503764E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3701</c:v>
+                  <c:v>3.6515513126491645E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3630</c:v>
+                  <c:v>5.4084014002333722E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3722</c:v>
+                  <c:v>5.3141285466126232E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3636</c:v>
+                  <c:v>5.3282182438192671E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1352,22 +1366,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>280</c:v>
+                  <c:v>7.4384942075239363E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>274</c:v>
+                  <c:v>1.4638099579597832E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>277</c:v>
+                  <c:v>3.1065088757396447E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>273</c:v>
+                  <c:v>4.4052863436123351E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>309</c:v>
+                  <c:v>4.1481069042316255E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>303</c:v>
+                  <c:v>4.3611111111111109E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1451,22 +1465,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>8.8156767921011533E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>1.5095858702762542E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>3.0305992765666241E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>5.0661412890515054E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>4.3368774482372695E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29</c:v>
+                  <c:v>3.3524235228383854E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,22 +1564,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5.0212146318194372E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>1.5100417778225197E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>4.6202180742931065E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>5.6793979838137155E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>2.7766208524226016E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>5.5850321139346547E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1739,7 +1753,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Committed Transactions</a:t>
+                  <a:t>Ops/sec</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2031,22 +2045,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3662</c:v>
+                  <c:v>1.2921485726265767E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3688</c:v>
+                  <c:v>2.5857223159078132E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3721</c:v>
+                  <c:v>5.0013583265417008E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3696</c:v>
+                  <c:v>7.1718146718146723E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3633</c:v>
+                  <c:v>7.0412056466997324E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3668</c:v>
+                  <c:v>7.1384076309129847E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2130,22 +2144,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>85</c:v>
+                  <c:v>3.511089480636863E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>6.9261670591494665E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81</c:v>
+                  <c:v>1.4298954057990202E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89</c:v>
+                  <c:v>1.9031781226903177E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93</c:v>
+                  <c:v>1.4614541468761417E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95</c:v>
+                  <c:v>2.1177781906000373E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2229,22 +2243,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>1.379167672309761E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>2.0787139689578713E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>2.6613439787092481E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>3.7509377344336085E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1.1273957158962797E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>7.4990626171728535E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2328,22 +2342,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2517,7 +2531,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Committed Transactions</a:t>
+                  <a:t>Ops/sec</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4707,29 +4721,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M59"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11">
@@ -4774,40 +4797,52 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>3746</v>
+        <f>'Raw Data'!B25</f>
+        <v>1.0943286193322642E-4</v>
       </c>
       <c r="C3" s="4">
-        <v>194</v>
+        <f>'Raw Data'!C25</f>
+        <v>5.6526504008767373E-6</v>
       </c>
       <c r="D3" s="4">
-        <v>14</v>
+        <f>'Raw Data'!D25</f>
+        <v>4.5722123792650169E-7</v>
       </c>
       <c r="E3" s="5">
-        <v>1</v>
+        <f>'Raw Data'!E25</f>
+        <v>8.5918034195377605E-8</v>
       </c>
       <c r="F3" s="3">
-        <v>3690</v>
+        <f>'Raw Data'!F25</f>
+        <v>9.5716471188169296E-5</v>
       </c>
       <c r="G3" s="4">
-        <v>280</v>
+        <f>'Raw Data'!G25</f>
+        <v>7.4384942075239363E-6</v>
       </c>
       <c r="H3" s="4">
-        <v>38</v>
+        <f>'Raw Data'!H25</f>
+        <v>8.8156767921011533E-7</v>
       </c>
       <c r="I3" s="5">
-        <v>3</v>
+        <f>'Raw Data'!I25</f>
+        <v>5.0212146318194372E-8</v>
       </c>
       <c r="J3" s="3">
-        <v>3662</v>
+        <f>'Raw Data'!J25</f>
+        <v>1.2921485726265767E-4</v>
       </c>
       <c r="K3" s="4">
-        <v>85</v>
+        <f>'Raw Data'!K25</f>
+        <v>3.511089480636863E-6</v>
       </c>
       <c r="L3" s="4">
-        <v>7</v>
+        <f>'Raw Data'!L25</f>
+        <v>1.379167672309761E-7</v>
       </c>
       <c r="M3" s="16">
-        <v>1</v>
+        <f>'Raw Data'!M25</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -4815,40 +4850,52 @@
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>3661</v>
+        <f>'Raw Data'!B26</f>
+        <v>2.1766045669567249E-4</v>
       </c>
       <c r="C4" s="2">
-        <v>208</v>
+        <f>'Raw Data'!C26</f>
+        <v>1.277550785521091E-5</v>
       </c>
       <c r="D4" s="2">
-        <v>16</v>
+        <f>'Raw Data'!D26</f>
+        <v>8.6137590444469967E-7</v>
       </c>
       <c r="E4" s="7">
-        <v>4</v>
+        <f>'Raw Data'!E26</f>
+        <v>1.7029006073678833E-7</v>
       </c>
       <c r="F4" s="6">
-        <v>3753</v>
+        <f>'Raw Data'!F26</f>
+        <v>1.9041523731503764E-4</v>
       </c>
       <c r="G4" s="2">
-        <v>274</v>
+        <f>'Raw Data'!G26</f>
+        <v>1.4638099579597832E-5</v>
       </c>
       <c r="H4" s="2">
-        <v>36</v>
+        <f>'Raw Data'!H26</f>
+        <v>1.5095858702762542E-6</v>
       </c>
       <c r="I4" s="7">
-        <v>4</v>
+        <f>'Raw Data'!I26</f>
+        <v>1.5100417778225197E-7</v>
       </c>
       <c r="J4" s="6">
-        <v>3688</v>
+        <f>'Raw Data'!J26</f>
+        <v>2.5857223159078132E-4</v>
       </c>
       <c r="K4" s="2">
-        <v>100</v>
+        <f>'Raw Data'!K26</f>
+        <v>6.9261670591494665E-6</v>
       </c>
       <c r="L4" s="2">
-        <v>5</v>
+        <f>'Raw Data'!L26</f>
+        <v>2.0787139689578713E-7</v>
       </c>
       <c r="M4" s="17">
-        <v>1</v>
+        <f>'Raw Data'!M26</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -4856,40 +4903,52 @@
         <v>4</v>
       </c>
       <c r="B5" s="6">
-        <v>3707</v>
+        <f>'Raw Data'!B27</f>
+        <v>4.1319638271742769E-4</v>
       </c>
       <c r="C5" s="2">
-        <v>185</v>
+        <f>'Raw Data'!C27</f>
+        <v>2.3294143500714208E-5</v>
       </c>
       <c r="D5" s="2">
-        <v>13</v>
+        <f>'Raw Data'!D27</f>
+        <v>2.6645942045076053E-6</v>
       </c>
       <c r="E5" s="7">
-        <v>3</v>
+        <f>'Raw Data'!E27</f>
+        <v>2.2070183182520415E-7</v>
       </c>
       <c r="F5" s="6">
-        <v>3701</v>
+        <f>'Raw Data'!F27</f>
+        <v>3.6515513126491645E-4</v>
       </c>
       <c r="G5" s="2">
-        <v>277</v>
+        <f>'Raw Data'!G27</f>
+        <v>3.1065088757396447E-5</v>
       </c>
       <c r="H5" s="2">
-        <v>33</v>
+        <f>'Raw Data'!H27</f>
+        <v>3.0305992765666241E-6</v>
       </c>
       <c r="I5" s="7">
-        <v>10</v>
+        <f>'Raw Data'!I27</f>
+        <v>4.6202180742931065E-7</v>
       </c>
       <c r="J5" s="6">
-        <v>3721</v>
+        <f>'Raw Data'!J27</f>
+        <v>5.0013583265417008E-4</v>
       </c>
       <c r="K5" s="2">
-        <v>81</v>
+        <f>'Raw Data'!K27</f>
+        <v>1.4298954057990202E-5</v>
       </c>
       <c r="L5" s="2">
-        <v>5</v>
+        <f>'Raw Data'!L27</f>
+        <v>2.6613439787092481E-7</v>
       </c>
       <c r="M5" s="17">
-        <v>1</v>
+        <f>'Raw Data'!M27</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -4897,40 +4956,52 @@
         <v>8</v>
       </c>
       <c r="B6" s="6">
-        <v>3760</v>
+        <f>'Raw Data'!B28</f>
+        <v>5.9228295819935696E-4</v>
       </c>
       <c r="C6" s="2">
-        <v>180</v>
+        <f>'Raw Data'!C28</f>
+        <v>3.0574428659666461E-5</v>
       </c>
       <c r="D6" s="2">
-        <v>22</v>
+        <f>'Raw Data'!D28</f>
+        <v>3.2185387833923397E-6</v>
       </c>
       <c r="E6" s="7">
-        <v>1</v>
+        <f>'Raw Data'!E28</f>
+        <v>3.2690421706440012E-7</v>
       </c>
       <c r="F6" s="6">
-        <v>3630</v>
+        <f>'Raw Data'!F28</f>
+        <v>5.4084014002333722E-4</v>
       </c>
       <c r="G6" s="2">
-        <v>273</v>
+        <f>'Raw Data'!G28</f>
+        <v>4.4052863436123351E-5</v>
       </c>
       <c r="H6" s="2">
-        <v>32</v>
+        <f>'Raw Data'!H28</f>
+        <v>5.0661412890515054E-6</v>
       </c>
       <c r="I6" s="7">
-        <v>9</v>
+        <f>'Raw Data'!I28</f>
+        <v>5.6793979838137155E-7</v>
       </c>
       <c r="J6" s="6">
-        <v>3696</v>
+        <f>'Raw Data'!J28</f>
+        <v>7.1718146718146723E-4</v>
       </c>
       <c r="K6" s="2">
-        <v>89</v>
+        <f>'Raw Data'!K28</f>
+        <v>1.9031781226903177E-5</v>
       </c>
       <c r="L6" s="2">
-        <v>4</v>
+        <f>'Raw Data'!L28</f>
+        <v>3.7509377344336085E-7</v>
       </c>
       <c r="M6" s="17">
-        <v>1</v>
+        <f>'Raw Data'!M28</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -4938,40 +5009,52 @@
         <v>16</v>
       </c>
       <c r="B7" s="6">
-        <v>3727</v>
+        <f>'Raw Data'!B29</f>
+        <v>6.0121192269898464E-4</v>
       </c>
       <c r="C7" s="2">
-        <v>214</v>
+        <f>'Raw Data'!C29</f>
+        <v>3.2617218127646231E-5</v>
       </c>
       <c r="D7" s="2">
-        <v>22</v>
+        <f>'Raw Data'!D29</f>
+        <v>2.3151720944590216E-6</v>
       </c>
       <c r="E7" s="7">
-        <v>2</v>
+        <f>'Raw Data'!E29</f>
+        <v>6.449532408900355E-7</v>
       </c>
       <c r="F7" s="6">
-        <v>3722</v>
+        <f>'Raw Data'!F29</f>
+        <v>5.3141285466126232E-4</v>
       </c>
       <c r="G7" s="2">
-        <v>309</v>
+        <f>'Raw Data'!G29</f>
+        <v>4.1481069042316255E-5</v>
       </c>
       <c r="H7" s="2">
-        <v>31</v>
+        <f>'Raw Data'!H29</f>
+        <v>4.3368774482372695E-6</v>
       </c>
       <c r="I7" s="7">
-        <v>3</v>
+        <f>'Raw Data'!I29</f>
+        <v>2.7766208524226016E-7</v>
       </c>
       <c r="J7" s="6">
-        <v>3633</v>
+        <f>'Raw Data'!J29</f>
+        <v>7.0412056466997324E-4</v>
       </c>
       <c r="K7" s="2">
-        <v>93</v>
+        <f>'Raw Data'!K29</f>
+        <v>1.4614541468761417E-5</v>
       </c>
       <c r="L7" s="2">
-        <v>5</v>
+        <f>'Raw Data'!L29</f>
+        <v>1.1273957158962797E-6</v>
       </c>
       <c r="M7" s="17">
-        <v>1</v>
+        <f>'Raw Data'!M29</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4979,45 +5062,57 @@
         <v>32</v>
       </c>
       <c r="B8" s="8">
-        <v>3719</v>
+        <f>'Raw Data'!B30</f>
+        <v>6.1241065627030543E-4</v>
       </c>
       <c r="C8" s="9">
-        <v>187</v>
+        <f>'Raw Data'!C30</f>
+        <v>3.5912919116478629E-5</v>
       </c>
       <c r="D8" s="9">
-        <v>12</v>
+        <f>'Raw Data'!D30</f>
+        <v>2.6459143968871595E-6</v>
       </c>
       <c r="E8" s="10">
-        <v>2</v>
+        <f>'Raw Data'!E30</f>
+        <v>1.6020506247997438E-7</v>
       </c>
       <c r="F8" s="8">
-        <v>3636</v>
+        <f>'Raw Data'!F30</f>
+        <v>5.3282182438192671E-4</v>
       </c>
       <c r="G8" s="9">
-        <v>303</v>
+        <f>'Raw Data'!G30</f>
+        <v>4.3611111111111109E-5</v>
       </c>
       <c r="H8" s="9">
-        <v>29</v>
+        <f>'Raw Data'!H30</f>
+        <v>3.3524235228383854E-6</v>
       </c>
       <c r="I8" s="10">
-        <v>2</v>
+        <f>'Raw Data'!I30</f>
+        <v>5.5850321139346547E-7</v>
       </c>
       <c r="J8" s="8">
-        <v>3668</v>
+        <f>'Raw Data'!J30</f>
+        <v>7.1384076309129847E-4</v>
       </c>
       <c r="K8" s="9">
-        <v>95</v>
+        <f>'Raw Data'!K30</f>
+        <v>2.1177781906000373E-5</v>
       </c>
       <c r="L8" s="9">
-        <v>2</v>
+        <f>'Raw Data'!L30</f>
+        <v>7.4990626171728535E-7</v>
       </c>
       <c r="M8" s="18">
-        <v>1</v>
+        <f>'Raw Data'!M30</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
@@ -5026,17 +5121,17 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="21" t="s">
-        <v>17</v>
+      <c r="C13" s="20" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -5046,12 +5141,1037 @@
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:M31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12">
+        <v>2</v>
+      </c>
+      <c r="D4" s="12">
+        <v>3</v>
+      </c>
+      <c r="E4" s="13">
+        <v>4</v>
+      </c>
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12">
+        <v>2</v>
+      </c>
+      <c r="H4" s="12">
+        <v>3</v>
+      </c>
+      <c r="I4" s="13">
+        <v>4</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1</v>
+      </c>
+      <c r="K4" s="12">
+        <v>2</v>
+      </c>
+      <c r="L4" s="12">
+        <v>3</v>
+      </c>
+      <c r="M4" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>34295</v>
+      </c>
+      <c r="C5" s="4">
+        <v>34674</v>
+      </c>
+      <c r="D5" s="4">
+        <v>34994</v>
+      </c>
+      <c r="E5" s="5">
+        <v>34917</v>
+      </c>
+      <c r="F5" s="3">
+        <v>39220</v>
+      </c>
+      <c r="G5" s="4">
+        <v>39793</v>
+      </c>
+      <c r="H5" s="4">
+        <v>39702</v>
+      </c>
+      <c r="I5" s="5">
+        <v>39831</v>
+      </c>
+      <c r="J5" s="3">
+        <v>28619</v>
+      </c>
+      <c r="K5" s="4">
+        <v>28766</v>
+      </c>
+      <c r="L5" s="4">
+        <v>29003</v>
+      </c>
+      <c r="M5" s="16">
+        <v>28931</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>17123</v>
+      </c>
+      <c r="C6" s="2">
+        <v>17377</v>
+      </c>
+      <c r="D6" s="2">
+        <v>17414</v>
+      </c>
+      <c r="E6" s="7">
+        <v>17617</v>
+      </c>
+      <c r="F6" s="6">
+        <v>19531</v>
+      </c>
+      <c r="G6" s="2">
+        <v>19743</v>
+      </c>
+      <c r="H6" s="2">
+        <v>19873</v>
+      </c>
+      <c r="I6" s="7">
+        <v>19867</v>
+      </c>
+      <c r="J6" s="6">
+        <v>14232</v>
+      </c>
+      <c r="K6" s="2">
+        <v>14438</v>
+      </c>
+      <c r="L6" s="2">
+        <v>14432</v>
+      </c>
+      <c r="M6" s="17">
+        <v>14545</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6">
+        <v>8957</v>
+      </c>
+      <c r="C7" s="2">
+        <v>9101</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9007</v>
+      </c>
+      <c r="E7" s="22">
+        <v>9062</v>
+      </c>
+      <c r="F7" s="6">
+        <v>10056</v>
+      </c>
+      <c r="G7" s="2">
+        <v>10140</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10229</v>
+      </c>
+      <c r="I7" s="7">
+        <v>10822</v>
+      </c>
+      <c r="J7" s="6">
+        <v>7362</v>
+      </c>
+      <c r="K7" s="2">
+        <v>7553</v>
+      </c>
+      <c r="L7" s="2">
+        <v>7515</v>
+      </c>
+      <c r="M7" s="17">
+        <v>7552</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>6220</v>
+      </c>
+      <c r="C8" s="2">
+        <v>6476</v>
+      </c>
+      <c r="D8" s="2">
+        <v>6214</v>
+      </c>
+      <c r="E8" s="7">
+        <v>6118</v>
+      </c>
+      <c r="F8" s="6">
+        <v>6856</v>
+      </c>
+      <c r="G8" s="2">
+        <v>7037</v>
+      </c>
+      <c r="H8" s="2">
+        <v>7106</v>
+      </c>
+      <c r="I8" s="7">
+        <v>7043</v>
+      </c>
+      <c r="J8" s="6">
+        <v>5180</v>
+      </c>
+      <c r="K8" s="2">
+        <v>5412</v>
+      </c>
+      <c r="L8" s="2">
+        <v>5332</v>
+      </c>
+      <c r="M8" s="17">
+        <v>5305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>16</v>
+      </c>
+      <c r="B9" s="6">
+        <v>6106</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6377</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6479</v>
+      </c>
+      <c r="E9" s="7">
+        <v>6202</v>
+      </c>
+      <c r="F9" s="6">
+        <v>6908</v>
+      </c>
+      <c r="G9" s="2">
+        <v>7184</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7148</v>
+      </c>
+      <c r="I9" s="7">
+        <v>7203</v>
+      </c>
+      <c r="J9" s="6">
+        <v>5242</v>
+      </c>
+      <c r="K9" s="2">
+        <v>5474</v>
+      </c>
+      <c r="L9" s="2">
+        <v>5322</v>
+      </c>
+      <c r="M9" s="17">
+        <v>5608</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>32</v>
+      </c>
+      <c r="B10" s="8">
+        <v>6156</v>
+      </c>
+      <c r="C10" s="9">
+        <v>6293</v>
+      </c>
+      <c r="D10" s="9">
+        <v>6425</v>
+      </c>
+      <c r="E10" s="10">
+        <v>6242</v>
+      </c>
+      <c r="F10" s="8">
+        <v>7038</v>
+      </c>
+      <c r="G10" s="9">
+        <v>7200</v>
+      </c>
+      <c r="H10" s="9">
+        <v>7159</v>
+      </c>
+      <c r="I10" s="10">
+        <v>7162</v>
+      </c>
+      <c r="J10" s="8">
+        <v>5137</v>
+      </c>
+      <c r="K10" s="9">
+        <v>5383</v>
+      </c>
+      <c r="L10" s="9">
+        <v>5334</v>
+      </c>
+      <c r="M10" s="18">
+        <v>5508</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12">
+        <v>2</v>
+      </c>
+      <c r="D14" s="12">
+        <v>3</v>
+      </c>
+      <c r="E14" s="13">
+        <v>4</v>
+      </c>
+      <c r="F14" s="11">
+        <v>1</v>
+      </c>
+      <c r="G14" s="12">
+        <v>2</v>
+      </c>
+      <c r="H14" s="12">
+        <v>3</v>
+      </c>
+      <c r="I14" s="13">
+        <v>4</v>
+      </c>
+      <c r="J14" s="11">
+        <v>1</v>
+      </c>
+      <c r="K14" s="12">
+        <v>2</v>
+      </c>
+      <c r="L14" s="12">
+        <v>3</v>
+      </c>
+      <c r="M14" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <v>3753</v>
+      </c>
+      <c r="C15" s="4">
+        <v>196</v>
+      </c>
+      <c r="D15" s="4">
+        <v>16</v>
+      </c>
+      <c r="E15" s="5">
+        <v>3</v>
+      </c>
+      <c r="F15" s="3">
+        <v>3754</v>
+      </c>
+      <c r="G15" s="4">
+        <v>296</v>
+      </c>
+      <c r="H15" s="4">
+        <v>35</v>
+      </c>
+      <c r="I15" s="5">
+        <v>2</v>
+      </c>
+      <c r="J15" s="3">
+        <v>3698</v>
+      </c>
+      <c r="K15" s="4">
+        <v>101</v>
+      </c>
+      <c r="L15" s="4">
+        <v>4</v>
+      </c>
+      <c r="M15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>2</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3727</v>
+      </c>
+      <c r="C16" s="2">
+        <v>222</v>
+      </c>
+      <c r="D16" s="2">
+        <v>15</v>
+      </c>
+      <c r="E16" s="7">
+        <v>3</v>
+      </c>
+      <c r="F16" s="6">
+        <v>3719</v>
+      </c>
+      <c r="G16" s="2">
+        <v>289</v>
+      </c>
+      <c r="H16" s="2">
+        <v>30</v>
+      </c>
+      <c r="I16" s="7">
+        <v>3</v>
+      </c>
+      <c r="J16" s="6">
+        <v>3680</v>
+      </c>
+      <c r="K16" s="2">
+        <v>100</v>
+      </c>
+      <c r="L16" s="2">
+        <v>3</v>
+      </c>
+      <c r="M16" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>4</v>
+      </c>
+      <c r="B17" s="6">
+        <v>3701</v>
+      </c>
+      <c r="C17" s="2">
+        <v>212</v>
+      </c>
+      <c r="D17" s="2">
+        <v>24</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2</v>
+      </c>
+      <c r="F17" s="6">
+        <v>3672</v>
+      </c>
+      <c r="G17" s="2">
+        <v>315</v>
+      </c>
+      <c r="H17" s="2">
+        <v>31</v>
+      </c>
+      <c r="I17" s="7">
+        <v>5</v>
+      </c>
+      <c r="J17" s="6">
+        <v>3682</v>
+      </c>
+      <c r="K17" s="2">
+        <v>108</v>
+      </c>
+      <c r="L17" s="2">
+        <v>2</v>
+      </c>
+      <c r="M17" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>8</v>
+      </c>
+      <c r="B18" s="6">
+        <v>3684</v>
+      </c>
+      <c r="C18" s="2">
+        <v>198</v>
+      </c>
+      <c r="D18" s="2">
+        <v>20</v>
+      </c>
+      <c r="E18" s="7">
+        <v>2</v>
+      </c>
+      <c r="F18" s="6">
+        <v>3708</v>
+      </c>
+      <c r="G18" s="2">
+        <v>310</v>
+      </c>
+      <c r="H18" s="2">
+        <v>36</v>
+      </c>
+      <c r="I18" s="7">
+        <v>4</v>
+      </c>
+      <c r="J18" s="6">
+        <v>3715</v>
+      </c>
+      <c r="K18" s="2">
+        <v>103</v>
+      </c>
+      <c r="L18" s="2">
+        <v>2</v>
+      </c>
+      <c r="M18" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6">
+        <v>3671</v>
+      </c>
+      <c r="C19" s="2">
+        <v>208</v>
+      </c>
+      <c r="D19" s="2">
+        <v>15</v>
+      </c>
+      <c r="E19" s="7">
+        <v>4</v>
+      </c>
+      <c r="F19" s="6">
+        <v>3671</v>
+      </c>
+      <c r="G19" s="2">
+        <v>298</v>
+      </c>
+      <c r="H19" s="2">
+        <v>31</v>
+      </c>
+      <c r="I19" s="7">
+        <v>2</v>
+      </c>
+      <c r="J19" s="6">
+        <v>3691</v>
+      </c>
+      <c r="K19" s="2">
+        <v>80</v>
+      </c>
+      <c r="L19" s="2">
+        <v>6</v>
+      </c>
+      <c r="M19" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
+        <v>32</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3770</v>
+      </c>
+      <c r="C20" s="9">
+        <v>226</v>
+      </c>
+      <c r="D20" s="9">
+        <v>17</v>
+      </c>
+      <c r="E20" s="10">
+        <v>1</v>
+      </c>
+      <c r="F20" s="8">
+        <v>3750</v>
+      </c>
+      <c r="G20" s="9">
+        <v>314</v>
+      </c>
+      <c r="H20" s="9">
+        <v>24</v>
+      </c>
+      <c r="I20" s="10">
+        <v>4</v>
+      </c>
+      <c r="J20" s="8">
+        <v>3667</v>
+      </c>
+      <c r="K20" s="9">
+        <v>114</v>
+      </c>
+      <c r="L20" s="9">
+        <v>4</v>
+      </c>
+      <c r="M20" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="11">
+        <v>1</v>
+      </c>
+      <c r="C24" s="12">
+        <v>2</v>
+      </c>
+      <c r="D24" s="12">
+        <v>3</v>
+      </c>
+      <c r="E24" s="13">
+        <v>4</v>
+      </c>
+      <c r="F24" s="11">
+        <v>1</v>
+      </c>
+      <c r="G24" s="12">
+        <v>2</v>
+      </c>
+      <c r="H24" s="12">
+        <v>3</v>
+      </c>
+      <c r="I24" s="13">
+        <v>4</v>
+      </c>
+      <c r="J24" s="11">
+        <v>1</v>
+      </c>
+      <c r="K24" s="12">
+        <v>2</v>
+      </c>
+      <c r="L24" s="12">
+        <v>3</v>
+      </c>
+      <c r="M24" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3">
+        <f>B15/(1000*B5)</f>
+        <v>1.0943286193322642E-4</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" ref="C25:M25" si="0">C15/(1000*C5)</f>
+        <v>5.6526504008767373E-6</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>4.5722123792650169E-7</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="0"/>
+        <v>8.5918034195377605E-8</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="0"/>
+        <v>9.5716471188169296E-5</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="0"/>
+        <v>7.4384942075239363E-6</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="0"/>
+        <v>8.8156767921011533E-7</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" si="0"/>
+        <v>5.0212146318194372E-8</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2921485726265767E-4</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="0"/>
+        <v>3.511089480636863E-6</v>
+      </c>
+      <c r="L25" s="4">
+        <f t="shared" si="0"/>
+        <v>1.379167672309761E-7</v>
+      </c>
+      <c r="M25" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>2</v>
+      </c>
+      <c r="B26" s="6">
+        <f t="shared" ref="B26:M26" si="1">B16/(1000*B6)</f>
+        <v>2.1766045669567249E-4</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="1"/>
+        <v>1.277550785521091E-5</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="1"/>
+        <v>8.6137590444469967E-7</v>
+      </c>
+      <c r="E26" s="7">
+        <f>E16/(1000*E6)</f>
+        <v>1.7029006073678833E-7</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="1"/>
+        <v>1.9041523731503764E-4</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4638099579597832E-5</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5095858702762542E-6</v>
+      </c>
+      <c r="I26" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5100417778225197E-7</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5857223159078132E-4</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="1"/>
+        <v>6.9261670591494665E-6</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0787139689578713E-7</v>
+      </c>
+      <c r="M26" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>4</v>
+      </c>
+      <c r="B27" s="6">
+        <f t="shared" ref="B27:M27" si="2">B17/(1000*B7)</f>
+        <v>4.1319638271742769E-4</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="2"/>
+        <v>2.3294143500714208E-5</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="2"/>
+        <v>2.6645942045076053E-6</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="2"/>
+        <v>2.2070183182520415E-7</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="2"/>
+        <v>3.6515513126491645E-4</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>3.1065088757396447E-5</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="2"/>
+        <v>3.0305992765666241E-6</v>
+      </c>
+      <c r="I27" s="7">
+        <f t="shared" si="2"/>
+        <v>4.6202180742931065E-7</v>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" si="2"/>
+        <v>5.0013583265417008E-4</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="2"/>
+        <v>1.4298954057990202E-5</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="2"/>
+        <v>2.6613439787092481E-7</v>
+      </c>
+      <c r="M27" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>8</v>
+      </c>
+      <c r="B28" s="6">
+        <f t="shared" ref="B28:M28" si="3">B18/(1000*B8)</f>
+        <v>5.9228295819935696E-4</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="3"/>
+        <v>3.0574428659666461E-5</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="3"/>
+        <v>3.2185387833923397E-6</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" si="3"/>
+        <v>3.2690421706440012E-7</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="3"/>
+        <v>5.4084014002333722E-4</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="3"/>
+        <v>4.4052863436123351E-5</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="3"/>
+        <v>5.0661412890515054E-6</v>
+      </c>
+      <c r="I28" s="7">
+        <f t="shared" si="3"/>
+        <v>5.6793979838137155E-7</v>
+      </c>
+      <c r="J28" s="6">
+        <f t="shared" si="3"/>
+        <v>7.1718146718146723E-4</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="3"/>
+        <v>1.9031781226903177E-5</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="3"/>
+        <v>3.7509377344336085E-7</v>
+      </c>
+      <c r="M28" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>16</v>
+      </c>
+      <c r="B29" s="6">
+        <f t="shared" ref="B29:M29" si="4">B19/(1000*B9)</f>
+        <v>6.0121192269898464E-4</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="4"/>
+        <v>3.2617218127646231E-5</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="4"/>
+        <v>2.3151720944590216E-6</v>
+      </c>
+      <c r="E29" s="7">
+        <f t="shared" si="4"/>
+        <v>6.449532408900355E-7</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" si="4"/>
+        <v>5.3141285466126232E-4</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="4"/>
+        <v>4.1481069042316255E-5</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="4"/>
+        <v>4.3368774482372695E-6</v>
+      </c>
+      <c r="I29" s="7">
+        <f t="shared" si="4"/>
+        <v>2.7766208524226016E-7</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" si="4"/>
+        <v>7.0412056466997324E-4</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="4"/>
+        <v>1.4614541468761417E-5</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="4"/>
+        <v>1.1273957158962797E-6</v>
+      </c>
+      <c r="M29" s="17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13">
+        <v>32</v>
+      </c>
+      <c r="B30" s="8">
+        <f t="shared" ref="B30:M30" si="5">B20/(1000*B10)</f>
+        <v>6.1241065627030543E-4</v>
+      </c>
+      <c r="C30" s="9">
+        <f t="shared" si="5"/>
+        <v>3.5912919116478629E-5</v>
+      </c>
+      <c r="D30" s="9">
+        <f t="shared" si="5"/>
+        <v>2.6459143968871595E-6</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="5"/>
+        <v>1.6020506247997438E-7</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" si="5"/>
+        <v>5.3282182438192671E-4</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="5"/>
+        <v>4.3611111111111109E-5</v>
+      </c>
+      <c r="H30" s="9">
+        <f t="shared" si="5"/>
+        <v>3.3524235228383854E-6</v>
+      </c>
+      <c r="I30" s="10">
+        <f t="shared" si="5"/>
+        <v>5.5850321139346547E-7</v>
+      </c>
+      <c r="J30" s="8">
+        <f t="shared" si="5"/>
+        <v>7.1384076309129847E-4</v>
+      </c>
+      <c r="K30" s="9">
+        <f t="shared" si="5"/>
+        <v>2.1177781906000373E-5</v>
+      </c>
+      <c r="L30" s="9">
+        <f t="shared" si="5"/>
+        <v>7.4990626171728535E-7</v>
+      </c>
+      <c r="M30" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Corrected code as per Lance's bug findings. Wiped out old benchmarks as they were computed using the buggy implementation.
</commit_message>
<xml_diff>
--- a/Assignments/Assignment3/Benchmarks.xlsx
+++ b/Assignments/Assignment3/Benchmarks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>1-32 threads</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Read dominated 4 operatrions per transaction had 0 successes, so it cannot appear on the logarithmic graph</t>
+  </si>
+  <si>
+    <t>&lt; Change this if you run it on a different PC</t>
   </si>
 </sst>
 </file>
@@ -314,10 +317,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -488,24 +491,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.0943286193322642E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.1766045669567249E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.1319638271742769E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.9228295819935696E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.0121192269898464E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.1241065627030543E-4</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -587,24 +572,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>5.6526504008767373E-6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.277550785521091E-5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.3294143500714208E-5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0574428659666461E-5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.2617218127646231E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.5912919116478629E-5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -686,24 +653,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4.5722123792650169E-7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.6137590444469967E-7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.6645942045076053E-6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.2185387833923397E-6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.3151720944590216E-6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.6459143968871595E-6</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -785,24 +734,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8.5918034195377605E-8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7029006073678833E-7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.2070183182520415E-7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.2690421706440012E-7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.449532408900355E-7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.6020506247997438E-7</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1266,24 +1197,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.5716471188169296E-5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9041523731503764E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.6515513126491645E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.4084014002333722E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.3141285466126232E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.3282182438192671E-4</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1365,24 +1278,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>7.4384942075239363E-6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.4638099579597832E-5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.1065088757396447E-5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.4052863436123351E-5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.1481069042316255E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.3611111111111109E-5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1464,24 +1359,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8.8156767921011533E-7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.5095858702762542E-6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0305992765666241E-6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0661412890515054E-6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.3368774482372695E-6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.3524235228383854E-6</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1563,24 +1440,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>5.0212146318194372E-8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.5100417778225197E-7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.6202180742931065E-7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.6793979838137155E-7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.7766208524226016E-7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.5850321139346547E-7</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2044,24 +1903,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.2921485726265767E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.5857223159078132E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0013583265417008E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.1718146718146723E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.0412056466997324E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.1384076309129847E-4</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2143,24 +1984,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3.511089480636863E-6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.9261670591494665E-6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4298954057990202E-5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.9031781226903177E-5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4614541468761417E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.1177781906000373E-5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2242,24 +2065,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.379167672309761E-7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0787139689578713E-7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.6613439787092481E-7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.7509377344336085E-7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1273957158962797E-6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.4990626171728535E-7</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2341,24 +2146,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4722,7 +4509,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M59"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4735,24 +4522,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11">
@@ -4796,319 +4583,103 @@
       <c r="A3" s="14">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <f>'Raw Data'!B25</f>
-        <v>1.0943286193322642E-4</v>
-      </c>
-      <c r="C3" s="4">
-        <f>'Raw Data'!C25</f>
-        <v>5.6526504008767373E-6</v>
-      </c>
-      <c r="D3" s="4">
-        <f>'Raw Data'!D25</f>
-        <v>4.5722123792650169E-7</v>
-      </c>
-      <c r="E3" s="5">
-        <f>'Raw Data'!E25</f>
-        <v>8.5918034195377605E-8</v>
-      </c>
-      <c r="F3" s="3">
-        <f>'Raw Data'!F25</f>
-        <v>9.5716471188169296E-5</v>
-      </c>
-      <c r="G3" s="4">
-        <f>'Raw Data'!G25</f>
-        <v>7.4384942075239363E-6</v>
-      </c>
-      <c r="H3" s="4">
-        <f>'Raw Data'!H25</f>
-        <v>8.8156767921011533E-7</v>
-      </c>
-      <c r="I3" s="5">
-        <f>'Raw Data'!I25</f>
-        <v>5.0212146318194372E-8</v>
-      </c>
-      <c r="J3" s="3">
-        <f>'Raw Data'!J25</f>
-        <v>1.2921485726265767E-4</v>
-      </c>
-      <c r="K3" s="4">
-        <f>'Raw Data'!K25</f>
-        <v>3.511089480636863E-6</v>
-      </c>
-      <c r="L3" s="4">
-        <f>'Raw Data'!L25</f>
-        <v>1.379167672309761E-7</v>
-      </c>
-      <c r="M3" s="16">
-        <f>'Raw Data'!M25</f>
-        <v>0</v>
-      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
-        <f>'Raw Data'!B26</f>
-        <v>2.1766045669567249E-4</v>
-      </c>
-      <c r="C4" s="2">
-        <f>'Raw Data'!C26</f>
-        <v>1.277550785521091E-5</v>
-      </c>
-      <c r="D4" s="2">
-        <f>'Raw Data'!D26</f>
-        <v>8.6137590444469967E-7</v>
-      </c>
-      <c r="E4" s="7">
-        <f>'Raw Data'!E26</f>
-        <v>1.7029006073678833E-7</v>
-      </c>
-      <c r="F4" s="6">
-        <f>'Raw Data'!F26</f>
-        <v>1.9041523731503764E-4</v>
-      </c>
-      <c r="G4" s="2">
-        <f>'Raw Data'!G26</f>
-        <v>1.4638099579597832E-5</v>
-      </c>
-      <c r="H4" s="2">
-        <f>'Raw Data'!H26</f>
-        <v>1.5095858702762542E-6</v>
-      </c>
-      <c r="I4" s="7">
-        <f>'Raw Data'!I26</f>
-        <v>1.5100417778225197E-7</v>
-      </c>
-      <c r="J4" s="6">
-        <f>'Raw Data'!J26</f>
-        <v>2.5857223159078132E-4</v>
-      </c>
-      <c r="K4" s="2">
-        <f>'Raw Data'!K26</f>
-        <v>6.9261670591494665E-6</v>
-      </c>
-      <c r="L4" s="2">
-        <f>'Raw Data'!L26</f>
-        <v>2.0787139689578713E-7</v>
-      </c>
-      <c r="M4" s="17">
-        <f>'Raw Data'!M26</f>
-        <v>0</v>
-      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="17"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <f>'Raw Data'!B27</f>
-        <v>4.1319638271742769E-4</v>
-      </c>
-      <c r="C5" s="2">
-        <f>'Raw Data'!C27</f>
-        <v>2.3294143500714208E-5</v>
-      </c>
-      <c r="D5" s="2">
-        <f>'Raw Data'!D27</f>
-        <v>2.6645942045076053E-6</v>
-      </c>
-      <c r="E5" s="7">
-        <f>'Raw Data'!E27</f>
-        <v>2.2070183182520415E-7</v>
-      </c>
-      <c r="F5" s="6">
-        <f>'Raw Data'!F27</f>
-        <v>3.6515513126491645E-4</v>
-      </c>
-      <c r="G5" s="2">
-        <f>'Raw Data'!G27</f>
-        <v>3.1065088757396447E-5</v>
-      </c>
-      <c r="H5" s="2">
-        <f>'Raw Data'!H27</f>
-        <v>3.0305992765666241E-6</v>
-      </c>
-      <c r="I5" s="7">
-        <f>'Raw Data'!I27</f>
-        <v>4.6202180742931065E-7</v>
-      </c>
-      <c r="J5" s="6">
-        <f>'Raw Data'!J27</f>
-        <v>5.0013583265417008E-4</v>
-      </c>
-      <c r="K5" s="2">
-        <f>'Raw Data'!K27</f>
-        <v>1.4298954057990202E-5</v>
-      </c>
-      <c r="L5" s="2">
-        <f>'Raw Data'!L27</f>
-        <v>2.6613439787092481E-7</v>
-      </c>
-      <c r="M5" s="17">
-        <f>'Raw Data'!M27</f>
-        <v>0</v>
-      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="17"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>8</v>
       </c>
-      <c r="B6" s="6">
-        <f>'Raw Data'!B28</f>
-        <v>5.9228295819935696E-4</v>
-      </c>
-      <c r="C6" s="2">
-        <f>'Raw Data'!C28</f>
-        <v>3.0574428659666461E-5</v>
-      </c>
-      <c r="D6" s="2">
-        <f>'Raw Data'!D28</f>
-        <v>3.2185387833923397E-6</v>
-      </c>
-      <c r="E6" s="7">
-        <f>'Raw Data'!E28</f>
-        <v>3.2690421706440012E-7</v>
-      </c>
-      <c r="F6" s="6">
-        <f>'Raw Data'!F28</f>
-        <v>5.4084014002333722E-4</v>
-      </c>
-      <c r="G6" s="2">
-        <f>'Raw Data'!G28</f>
-        <v>4.4052863436123351E-5</v>
-      </c>
-      <c r="H6" s="2">
-        <f>'Raw Data'!H28</f>
-        <v>5.0661412890515054E-6</v>
-      </c>
-      <c r="I6" s="7">
-        <f>'Raw Data'!I28</f>
-        <v>5.6793979838137155E-7</v>
-      </c>
-      <c r="J6" s="6">
-        <f>'Raw Data'!J28</f>
-        <v>7.1718146718146723E-4</v>
-      </c>
-      <c r="K6" s="2">
-        <f>'Raw Data'!K28</f>
-        <v>1.9031781226903177E-5</v>
-      </c>
-      <c r="L6" s="2">
-        <f>'Raw Data'!L28</f>
-        <v>3.7509377344336085E-7</v>
-      </c>
-      <c r="M6" s="17">
-        <f>'Raw Data'!M28</f>
-        <v>0</v>
-      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="17"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>16</v>
       </c>
-      <c r="B7" s="6">
-        <f>'Raw Data'!B29</f>
-        <v>6.0121192269898464E-4</v>
-      </c>
-      <c r="C7" s="2">
-        <f>'Raw Data'!C29</f>
-        <v>3.2617218127646231E-5</v>
-      </c>
-      <c r="D7" s="2">
-        <f>'Raw Data'!D29</f>
-        <v>2.3151720944590216E-6</v>
-      </c>
-      <c r="E7" s="7">
-        <f>'Raw Data'!E29</f>
-        <v>6.449532408900355E-7</v>
-      </c>
-      <c r="F7" s="6">
-        <f>'Raw Data'!F29</f>
-        <v>5.3141285466126232E-4</v>
-      </c>
-      <c r="G7" s="2">
-        <f>'Raw Data'!G29</f>
-        <v>4.1481069042316255E-5</v>
-      </c>
-      <c r="H7" s="2">
-        <f>'Raw Data'!H29</f>
-        <v>4.3368774482372695E-6</v>
-      </c>
-      <c r="I7" s="7">
-        <f>'Raw Data'!I29</f>
-        <v>2.7766208524226016E-7</v>
-      </c>
-      <c r="J7" s="6">
-        <f>'Raw Data'!J29</f>
-        <v>7.0412056466997324E-4</v>
-      </c>
-      <c r="K7" s="2">
-        <f>'Raw Data'!K29</f>
-        <v>1.4614541468761417E-5</v>
-      </c>
-      <c r="L7" s="2">
-        <f>'Raw Data'!L29</f>
-        <v>1.1273957158962797E-6</v>
-      </c>
-      <c r="M7" s="17">
-        <f>'Raw Data'!M29</f>
-        <v>0</v>
-      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>32</v>
       </c>
-      <c r="B8" s="8">
-        <f>'Raw Data'!B30</f>
-        <v>6.1241065627030543E-4</v>
-      </c>
-      <c r="C8" s="9">
-        <f>'Raw Data'!C30</f>
-        <v>3.5912919116478629E-5</v>
-      </c>
-      <c r="D8" s="9">
-        <f>'Raw Data'!D30</f>
-        <v>2.6459143968871595E-6</v>
-      </c>
-      <c r="E8" s="10">
-        <f>'Raw Data'!E30</f>
-        <v>1.6020506247997438E-7</v>
-      </c>
-      <c r="F8" s="8">
-        <f>'Raw Data'!F30</f>
-        <v>5.3282182438192671E-4</v>
-      </c>
-      <c r="G8" s="9">
-        <f>'Raw Data'!G30</f>
-        <v>4.3611111111111109E-5</v>
-      </c>
-      <c r="H8" s="9">
-        <f>'Raw Data'!H30</f>
-        <v>3.3524235228383854E-6</v>
-      </c>
-      <c r="I8" s="10">
-        <f>'Raw Data'!I30</f>
-        <v>5.5850321139346547E-7</v>
-      </c>
-      <c r="J8" s="8">
-        <f>'Raw Data'!J30</f>
-        <v>7.1384076309129847E-4</v>
-      </c>
-      <c r="K8" s="9">
-        <f>'Raw Data'!K30</f>
-        <v>2.1177781906000373E-5</v>
-      </c>
-      <c r="L8" s="9">
-        <f>'Raw Data'!L30</f>
-        <v>7.4990626171728535E-7</v>
-      </c>
-      <c r="M8" s="18">
-        <f>'Raw Data'!M30</f>
-        <v>0</v>
-      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="18"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -5117,6 +4688,9 @@
       </c>
       <c r="C10" t="s">
         <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -5160,24 +4734,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21" t="s">
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -5315,7 +4889,7 @@
       <c r="D7" s="2">
         <v>9007</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <v>9062</v>
       </c>
       <c r="F7" s="6">
@@ -5468,24 +5042,24 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21" t="s">
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21" t="s">
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -5776,24 +5350,24 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21" t="s">
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21" t="s">
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -6157,15 +5731,15 @@
     <row r="31" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="J13:M13"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="F23:I23"/>
     <mergeCell ref="J23:M23"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Re-format benchmark plottings to emphasize change and add Benchmarks PDF
</commit_message>
<xml_diff>
--- a/Assignments/Assignment3/Benchmarks.xlsx
+++ b/Assignments/Assignment3/Benchmarks.xlsx
@@ -945,7 +945,7 @@
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
           <c:max val="100000.0"/>
-          <c:min val="100.0"/>
+          <c:min val="1000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1729,7 +1729,7 @@
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
-          <c:min val="100.0"/>
+          <c:min val="1000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2512,7 +2512,7 @@
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
-          <c:min val="100.0"/>
+          <c:min val="1000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4744,7 +4744,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>